<commit_message>
made sheets match standard
</commit_message>
<xml_diff>
--- a/library/library_1476.xlsx
+++ b/library/library_1476.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC878E77-7113-7240-9FDD-004AAA2386BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE39575-2D34-A442-B43F-057146A6CF9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16700" yWindow="6640" windowWidth="14920" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>12.11.14</t>
   </si>
   <si>
-    <t>Retrofitted_1476</t>
-  </si>
-  <si>
     <t>02.16.15</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>TACTCTA</t>
+  </si>
+  <si>
+    <t>S.GISH</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -472,25 +472,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -498,25 +498,25 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -524,25 +524,25 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -550,25 +550,25 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -576,25 +576,25 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -602,25 +602,25 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>